<commit_message>
updated code for hardiks sql
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication1/sql formatter.xlsx
+++ b/WindowsFormsApplication1/sql formatter.xlsx
@@ -344,16 +344,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C77" sqref="C1:C77"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -361,692 +361,701 @@
         <v>0</v>
       </c>
       <c r="C1" t="str">
-        <f>CONCATENATE($A$1,B1,"+")</f>
-        <v>varname1+</v>
+        <f>CONCATENATE($A$1,B1,"+Environment.NewLine+")</f>
+        <v>varname1+Environment.NewLine+</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C65" si="0">CONCATENATE($A$1,B2,"+")</f>
-        <v>varname12+</v>
+        <f>CONCATENATE($A$1,B2,"+Environment.NewLine+")</f>
+        <v>varname11+Environment.NewLine+</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v>varname13+</v>
+        <f t="shared" ref="C3:C66" si="0">CONCATENATE($A$1,B3,"+Environment.NewLine+")</f>
+        <v>varname12+Environment.NewLine+</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>varname14+</v>
+        <v>varname13+Environment.NewLine+</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>varname15+</v>
+        <v>varname14+Environment.NewLine+</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>varname16+</v>
+        <v>varname15+Environment.NewLine+</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>varname17+</v>
+        <v>varname16+Environment.NewLine+</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>varname18+</v>
+        <v>varname17+Environment.NewLine+</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>varname19+</v>
+        <v>varname18+Environment.NewLine+</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>varname110+</v>
+        <v>varname19+Environment.NewLine+</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>varname111+</v>
+        <v>varname110+Environment.NewLine+</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>varname112+</v>
+        <v>varname111+Environment.NewLine+</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>varname113+</v>
+        <v>varname112+Environment.NewLine+</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>varname114+</v>
+        <v>varname113+Environment.NewLine+</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>varname115+</v>
+        <v>varname114+Environment.NewLine+</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>varname116+</v>
+        <v>varname115+Environment.NewLine+</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>varname117+</v>
+        <v>varname116+Environment.NewLine+</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>varname118+</v>
+        <v>varname117+Environment.NewLine+</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>varname119+</v>
+        <v>varname118+Environment.NewLine+</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>varname120+</v>
+        <v>varname119+Environment.NewLine+</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>varname121+</v>
+        <v>varname120+Environment.NewLine+</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>varname122+</v>
+        <v>varname121+Environment.NewLine+</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>varname123+</v>
+        <v>varname122+Environment.NewLine+</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>varname124+</v>
+        <v>varname123+Environment.NewLine+</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>varname125+</v>
+        <v>varname124+Environment.NewLine+</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>varname126+</v>
+        <v>varname125+Environment.NewLine+</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>varname127+</v>
+        <v>varname126+Environment.NewLine+</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>varname128+</v>
+        <v>varname127+Environment.NewLine+</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>varname129+</v>
+        <v>varname128+Environment.NewLine+</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>varname130+</v>
+        <v>varname129+Environment.NewLine+</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>varname131+</v>
+        <v>varname130+Environment.NewLine+</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>varname132+</v>
+        <v>varname131+Environment.NewLine+</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>varname133+</v>
+        <v>varname132+Environment.NewLine+</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>varname134+</v>
+        <v>varname133+Environment.NewLine+</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>varname135+</v>
+        <v>varname134+Environment.NewLine+</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>varname136+</v>
+        <v>varname135+Environment.NewLine+</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>varname137+</v>
+        <v>varname136+Environment.NewLine+</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>varname138+</v>
+        <v>varname137+Environment.NewLine+</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>varname139+</v>
+        <v>varname138+Environment.NewLine+</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>varname140+</v>
+        <v>varname139+Environment.NewLine+</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>varname141+</v>
+        <v>varname140+Environment.NewLine+</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>varname142+</v>
+        <v>varname141+Environment.NewLine+</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>varname143+</v>
+        <v>varname142+Environment.NewLine+</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>varname144+</v>
+        <v>varname143+Environment.NewLine+</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>varname145+</v>
+        <v>varname144+Environment.NewLine+</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>varname146+</v>
+        <v>varname145+Environment.NewLine+</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>varname147+</v>
+        <v>varname146+Environment.NewLine+</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>varname148+</v>
+        <v>varname147+Environment.NewLine+</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>varname149+</v>
+        <v>varname148+Environment.NewLine+</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>varname150+</v>
+        <v>varname149+Environment.NewLine+</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>varname151+</v>
+        <v>varname150+Environment.NewLine+</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>varname152+</v>
+        <v>varname151+Environment.NewLine+</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>varname153+</v>
+        <v>varname152+Environment.NewLine+</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>varname154+</v>
+        <v>varname153+Environment.NewLine+</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>varname155+</v>
+        <v>varname154+Environment.NewLine+</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>varname156+</v>
+        <v>varname155+Environment.NewLine+</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>varname157+</v>
+        <v>varname156+Environment.NewLine+</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>varname158+</v>
+        <v>varname157+Environment.NewLine+</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>varname159+</v>
+        <v>varname158+Environment.NewLine+</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>varname160+</v>
+        <v>varname159+Environment.NewLine+</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>varname161+</v>
+        <v>varname160+Environment.NewLine+</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>varname162+</v>
+        <v>varname161+Environment.NewLine+</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>varname163+</v>
+        <v>varname162+Environment.NewLine+</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>varname164+</v>
+        <v>varname163+Environment.NewLine+</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v>varname165+</v>
+        <v>varname164+Environment.NewLine+</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C77" si="1">CONCATENATE($A$1,B66,"+")</f>
-        <v>varname166+</v>
+        <f t="shared" si="0"/>
+        <v>varname165+Environment.NewLine+</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v>varname167+</v>
+        <f t="shared" ref="C67:C78" si="1">CONCATENATE($A$1,B67,"+Environment.NewLine+")</f>
+        <v>varname166+Environment.NewLine+</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v>varname168+</v>
+        <v>varname167+Environment.NewLine+</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v>varname169+</v>
+        <v>varname168+Environment.NewLine+</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v>varname170+</v>
+        <v>varname169+Environment.NewLine+</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>varname171+</v>
+        <v>varname170+Environment.NewLine+</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>varname172+</v>
+        <v>varname171+Environment.NewLine+</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>varname173+</v>
+        <v>varname172+Environment.NewLine+</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v>varname174+</v>
+        <v>varname173+Environment.NewLine+</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v>varname175+</v>
+        <v>varname174+Environment.NewLine+</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>varname176+</v>
+        <v>varname175+Environment.NewLine+</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>varname177+</v>
+        <v>varname176+Environment.NewLine+</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>varname177+Environment.NewLine+</v>
       </c>
     </row>
   </sheetData>

</xml_diff>